<commit_message>
20160415 commit new code
</commit_message>
<xml_diff>
--- a/IPCV7testing/IPC_v7_message.xlsx
+++ b/IPCV7testing/IPC_v7_message.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -221,6 +221,22 @@
   </si>
   <si>
     <t>50hz</t>
+  </si>
+  <si>
+    <t>增益上限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -858,10 +874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1065,16 +1081,16 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
+        <v>54</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1090,17 +1106,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>17</v>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1115,15 +1131,18 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -1140,48 +1159,22 @@
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q11" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
@@ -1189,30 +1182,66 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>52</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1339,6 +1368,19 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>